<commit_message>
fixed isweakly for checking all coefficients
</commit_message>
<xml_diff>
--- a/wi-polynomial-w-firstcoef-results-2,3.xlsx
+++ b/wi-polynomial-w-firstcoef-results-2,3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>p^3</t>
   </si>
@@ -27,34 +27,34 @@
     <t>p^5</t>
   </si>
   <si>
-    <t>p^6</t>
-  </si>
-  <si>
-    <t>p^7</t>
-  </si>
-  <si>
-    <t>p^8</t>
-  </si>
-  <si>
-    <t>p^9</t>
-  </si>
-  <si>
-    <t>p^10</t>
-  </si>
-  <si>
-    <t>p^11</t>
-  </si>
-  <si>
-    <t>p^12</t>
-  </si>
-  <si>
-    <t>p^13</t>
-  </si>
-  <si>
-    <t>p^14</t>
-  </si>
-  <si>
-    <t>p^15</t>
+    <t>[1, 1, 0, 1]</t>
+  </si>
+  <si>
+    <t>[1, 1, 0, 0, 1]</t>
+  </si>
+  <si>
+    <t>[1, 1, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>[1, 1, 0, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>[1, 1, 1, 0, 1, 1]</t>
+  </si>
+  <si>
+    <t>[1, 1, 1, 1, 0, 1]</t>
+  </si>
+  <si>
+    <t>[1, 1, 0, 1, 2, 2]</t>
+  </si>
+  <si>
+    <t>[1, 1, 2, 0, 2, 2]</t>
+  </si>
+  <si>
+    <t>[1, 2, 0, 2, 2, 1]</t>
+  </si>
+  <si>
+    <t>[1, 2, 2, 0, 2, 1]</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -405,7 +405,7 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -416,7 +416,7 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -427,120 +427,10 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
+        <v>0.07272727272727272</v>
       </c>
     </row>
   </sheetData>
@@ -550,7 +440,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -569,7 +459,7 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -580,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -591,120 +481,10 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
         <v>4</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -714,7 +494,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:C1"/>
+  <dimension ref="B1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -731,6 +511,48 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="2:3">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>